<commit_message>
ACT 2 OCT 2020
</commit_message>
<xml_diff>
--- a/CHILE/Agricultura/Emisiones CO2 Agricultura Chile 1990-2016.xlsx
+++ b/CHILE/Agricultura/Emisiones CO2 Agricultura Chile 1990-2016.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Arancibia\Dropbox\Diseño DATA's (1)\DATAICC\CHILE\Agricultura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Arancibia\Dropbox\Diseño DATA's (1)\DATA-ICC\CHILE\Agricultura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DE86AD6-933C-495B-AF22-DE1C6A3D1FE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EE08185-E085-4757-81B2-75627C96DEF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ark1 (2)" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Emisiones por Tipo de emisión</t>
   </si>
@@ -60,11 +61,32 @@
   <si>
     <t>Año</t>
   </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Proceso</t>
+  </si>
+  <si>
+    <t>Agricultura</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Emisiones (kton CO2)</t>
+  </si>
+  <si>
+    <t>Emisiones (kton CO2eq)</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -557,7 +579,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -565,13 +587,14 @@
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -617,7 +640,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="33">
     <dxf>
       <font>
         <b/>
@@ -635,12 +658,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -655,7 +678,68 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -897,6 +981,324 @@
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -911,21 +1313,47 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="CO2_Agricultura_Chile" displayName="CO2_Agricultura_Chile" ref="A2:L29" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A2:L29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="CO2_Agricultura_Chile" displayName="CO2_Agricultura_Chile" ref="A2:L29" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A2:L29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Año" dataDxfId="13"/>
-    <tableColumn id="2" name="3.A - Fermentación entérica" dataDxfId="12"/>
-    <tableColumn id="3" name="3.B - Gestión del estiércol" dataDxfId="11"/>
-    <tableColumn id="4" name="3.C - Cultivo del arroz" dataDxfId="10"/>
-    <tableColumn id="5" name="3.D - Suelos agrícolas" dataDxfId="9"/>
-    <tableColumn id="6" name="3.E - Quema prescrita de sabanas" dataDxfId="8"/>
-    <tableColumn id="7" name="3.F - Quema de residuos agrícola en el campo" dataDxfId="7"/>
-    <tableColumn id="8" name="3.G - Encalado" dataDxfId="6"/>
-    <tableColumn id="9" name="3.H - Aplicación de urea" dataDxfId="5"/>
-    <tableColumn id="10" name="3.I - Otros fertilizantes que contienen carbono" dataDxfId="4"/>
-    <tableColumn id="11" name="3.J - Otros" dataDxfId="3"/>
-    <tableColumn id="12" name="3 - Agricultura" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Año" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="3.A - Fermentación entérica" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="3.B - Gestión del estiércol" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="3.C - Cultivo del arroz" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="3.D - Suelos agrícolas" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="3.E - Quema prescrita de sabanas" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="3.F - Quema de residuos agrícola en el campo" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="3.G - Encalado" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="3.H - Aplicación de urea" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="3.I - Otros fertilizantes que contienen carbono" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="3.J - Otros" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="3 - Agricultura" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{542763A0-908A-4A86-B48C-F22A6103A71B}" name="CO2_Agricultura_Chile3" displayName="CO2_Agricultura_Chile3" ref="A2:Q29" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A2:Q29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{EDFE7A38-641B-494A-8910-C33A357024C3}" name="Año" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{02F8B638-4A46-4983-93C7-E44ECACBB250}" name="Sector" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{06A1A192-2A07-4AD1-83F1-4056BE6BB6C4}" name="Proceso" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{9C5D1406-D0EB-4EEA-AB79-84EEAE7339B4}" name="Gas" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{F445F3F8-4CF9-4B56-9A61-943541AA31F3}" name="Emisiones (kton CO2)" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{FD7EDAA8-04D6-4326-8AA5-B09E3FBF4DE1}" name="Emisiones (kton CO2eq)" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{30B917CA-F723-452C-B1F7-9193DC5C72D8}" name="3.A - Fermentación entérica" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{000B48AA-EAD8-463E-A0FF-31FC94CF69CF}" name="3.B - Gestión del estiércol" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{4F2FF258-13C9-4377-812A-E37BD5377073}" name="3.C - Cultivo del arroz" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{A271DEB9-A4D6-4EF4-93D6-C9013F567A65}" name="3.D - Suelos agrícolas" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{4FE4C99A-14C4-456B-BFDE-2CD6A98A79F3}" name="3.E - Quema prescrita de sabanas" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{443EFB26-280B-4235-89E7-08F47A1DCA44}" name="3.F - Quema de residuos agrícola en el campo" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{EBF0F9DE-280F-45BC-A74B-48F030E7EA29}" name="3.G - Encalado" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{925C0E2F-F0B8-4197-9D37-AAB0E75F6896}" name="3.H - Aplicación de urea" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{C08B8BE1-7C36-46A6-9651-841C77A1D56D}" name="3.I - Otros fertilizantes que contienen carbono" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{E4BCFDAC-C8CD-435A-B844-E393D9182887}" name="3.J - Otros" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{E1CFE338-2C15-405F-BF41-3A013543D7DC}" name="3 - Agricultura" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1227,14 +1655,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L29"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
@@ -1250,23 +1678,23 @@
     <col min="12" max="12" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1304,8 +1732,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>1990</v>
       </c>
       <c r="B3" s="2">
@@ -1342,8 +1770,8 @@
         <v>200.4697189</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>1991</v>
       </c>
       <c r="B4" s="2">
@@ -1380,8 +1808,8 @@
         <v>225.53105840000001</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>1992</v>
       </c>
       <c r="B5" s="2">
@@ -1418,8 +1846,8 @@
         <v>244.78105679999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>1993</v>
       </c>
       <c r="B6" s="2">
@@ -1456,8 +1884,8 @@
         <v>247.93048759999999</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>1994</v>
       </c>
       <c r="B7" s="2">
@@ -1494,8 +1922,8 @@
         <v>239.07130599999999</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>1995</v>
       </c>
       <c r="B8" s="2">
@@ -1532,8 +1960,8 @@
         <v>263.80488400000002</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>1996</v>
       </c>
       <c r="B9" s="2">
@@ -1570,8 +1998,8 @@
         <v>341.9600418</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>1997</v>
       </c>
       <c r="B10" s="2">
@@ -1608,8 +2036,8 @@
         <v>257.23057069999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>1998</v>
       </c>
       <c r="B11" s="2">
@@ -1646,8 +2074,8 @@
         <v>295.58223570000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>1999</v>
       </c>
       <c r="B12" s="2">
@@ -1684,8 +2112,8 @@
         <v>329.17047739999998</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>2000</v>
       </c>
       <c r="B13" s="2">
@@ -1722,8 +2150,8 @@
         <v>366.49522139999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>2001</v>
       </c>
       <c r="B14" s="2">
@@ -1760,8 +2188,8 @@
         <v>340.93321680000003</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>2002</v>
       </c>
       <c r="B15" s="2">
@@ -1798,8 +2226,8 @@
         <v>388.7820347</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>2003</v>
       </c>
       <c r="B16" s="2">
@@ -1836,8 +2264,8 @@
         <v>420.84577480000002</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>2004</v>
       </c>
       <c r="B17" s="2">
@@ -1874,8 +2302,8 @@
         <v>440.42806280000002</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>2005</v>
       </c>
       <c r="B18" s="2">
@@ -1912,8 +2340,8 @@
         <v>376.5409707</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>2006</v>
       </c>
       <c r="B19" s="2">
@@ -1950,8 +2378,8 @@
         <v>395.97669180000003</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>2007</v>
       </c>
       <c r="B20" s="2">
@@ -1988,8 +2416,8 @@
         <v>395.02162019999997</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>2008</v>
       </c>
       <c r="B21" s="2">
@@ -2026,8 +2454,8 @@
         <v>431.45542330000001</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>2009</v>
       </c>
       <c r="B22" s="2">
@@ -2064,8 +2492,8 @@
         <v>392.16879390000003</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>2010</v>
       </c>
       <c r="B23" s="2">
@@ -2102,8 +2530,8 @@
         <v>470.10858050000002</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>2011</v>
       </c>
       <c r="B24" s="2">
@@ -2140,8 +2568,8 @@
         <v>489.166338</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>2012</v>
       </c>
       <c r="B25" s="2">
@@ -2178,8 +2606,8 @@
         <v>485.50430920000002</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>2013</v>
       </c>
       <c r="B26" s="2">
@@ -2216,8 +2644,8 @@
         <v>509.32057789999999</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
         <v>2014</v>
       </c>
       <c r="B27" s="2">
@@ -2254,8 +2682,8 @@
         <v>481.72731190000002</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>2015</v>
       </c>
       <c r="B28" s="2">
@@ -2292,8 +2720,8 @@
         <v>528.0885356</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>2016</v>
       </c>
       <c r="B29" s="2">
@@ -2340,4 +2768,1287 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E52A6C1-D7DC-45CB-B73C-88F74BED2C6C}">
+  <dimension ref="A1:Q29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="23" style="3" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="38.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="39" style="3" customWidth="1"/>
+    <col min="16" max="16" width="11" style="3" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="3" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+    </row>
+    <row r="2" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1990</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>30.8</v>
+      </c>
+      <c r="N3" s="2">
+        <v>169.66971889999999</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>200.4697189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1991</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>33.131999999999998</v>
+      </c>
+      <c r="N4" s="2">
+        <v>192.3990584</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>225.53105840000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1992</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>35.463999999999999</v>
+      </c>
+      <c r="N5" s="2">
+        <v>209.31705679999999</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>244.78105679999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1993</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>37.795999999999999</v>
+      </c>
+      <c r="N6" s="2">
+        <v>210.1344876</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>247.93048759999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1994</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>40.128</v>
+      </c>
+      <c r="N7" s="2">
+        <v>198.94330600000001</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>239.07130599999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1995</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>41.052</v>
+      </c>
+      <c r="N8" s="2">
+        <v>222.75288399999999</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>263.80488400000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>1996</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>45.847999999999999</v>
+      </c>
+      <c r="N9" s="2">
+        <v>296.11204179999999</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>341.9600418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1997</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>50.951999999999998</v>
+      </c>
+      <c r="N10" s="2">
+        <v>206.27857069999999</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>257.23057069999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1998</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>58.695999999999998</v>
+      </c>
+      <c r="N11" s="2">
+        <v>236.88623569999999</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>295.58223570000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>1999</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>56.892000000000003</v>
+      </c>
+      <c r="N12" s="2">
+        <v>272.27847739999999</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>329.17047739999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>2000</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>63.624000000000002</v>
+      </c>
+      <c r="N13" s="2">
+        <v>302.87122140000002</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>366.49522139999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>2001</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>67.540000000000006</v>
+      </c>
+      <c r="N14" s="2">
+        <v>273.3932168</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>340.93321680000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2002</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>80.212000000000003</v>
+      </c>
+      <c r="N15" s="2">
+        <v>308.57003470000001</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>388.7820347</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2003</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2">
+        <v>77.66</v>
+      </c>
+      <c r="N16" s="2">
+        <v>343.18577479999999</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>420.84577480000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>2004</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>89.1</v>
+      </c>
+      <c r="N17" s="2">
+        <v>351.3280628</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>440.42806280000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2005</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2">
+        <v>81.326695999999998</v>
+      </c>
+      <c r="N18" s="2">
+        <v>295.21427469999998</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>376.5409707</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>2006</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2">
+        <v>83.9198624</v>
+      </c>
+      <c r="N19" s="2">
+        <v>312.05682940000003</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>395.97669180000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>2007</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2">
+        <v>86.372352000000006</v>
+      </c>
+      <c r="N20" s="2">
+        <v>308.64926819999999</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>395.02162019999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>2008</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2">
+        <v>88.684164800000005</v>
+      </c>
+      <c r="N21" s="2">
+        <v>342.77125849999999</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>431.45542330000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>2009</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2">
+        <v>90.855300799999995</v>
+      </c>
+      <c r="N22" s="2">
+        <v>301.31349310000002</v>
+      </c>
+      <c r="O22" s="2">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>392.16879390000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>2010</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2">
+        <v>92.885760000000005</v>
+      </c>
+      <c r="N23" s="2">
+        <v>377.22282050000001</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>470.10858050000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>2011</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2">
+        <v>115.3198757</v>
+      </c>
+      <c r="N24" s="2">
+        <v>373.84646229999998</v>
+      </c>
+      <c r="O24" s="2">
+        <v>0</v>
+      </c>
+      <c r="P24" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>489.166338</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>2012</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2">
+        <v>113.24165600000001</v>
+      </c>
+      <c r="N25" s="2">
+        <v>372.26265319999999</v>
+      </c>
+      <c r="O25" s="2">
+        <v>0</v>
+      </c>
+      <c r="P25" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>485.50430920000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>2013</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
+        <v>108.94537870000001</v>
+      </c>
+      <c r="N26" s="2">
+        <v>400.3751992</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0</v>
+      </c>
+      <c r="P26" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>509.32057789999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>2014</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2">
+        <v>100.24910130000001</v>
+      </c>
+      <c r="N27" s="2">
+        <v>381.47821060000001</v>
+      </c>
+      <c r="O27" s="2">
+        <v>0</v>
+      </c>
+      <c r="P27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>481.72731190000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>2015</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2">
+        <v>95.072823999999997</v>
+      </c>
+      <c r="N28" s="2">
+        <v>433.01571159999997</v>
+      </c>
+      <c r="O28" s="2">
+        <v>0</v>
+      </c>
+      <c r="P28" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>528.0885356</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>2016</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0</v>
+      </c>
+      <c r="M29" s="2">
+        <v>88.400546700000007</v>
+      </c>
+      <c r="N29" s="2">
+        <v>356.95122320000002</v>
+      </c>
+      <c r="O29" s="2">
+        <v>0</v>
+      </c>
+      <c r="P29" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>445.35176990000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Act 3 OCT 2020
</commit_message>
<xml_diff>
--- a/CHILE/Agricultura/Emisiones CO2 Agricultura Chile 1990-2016.xlsx
+++ b/CHILE/Agricultura/Emisiones CO2 Agricultura Chile 1990-2016.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Arancibia\Dropbox\Diseño DATA's (1)\DATA-ICC\CHILE\Agricultura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB26596-2DA6-44C4-B383-57603F1E1FB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A620A9E6-CB39-477E-880D-9908D691C642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,13 +597,13 @@
     <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -667,13 +667,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -778,26 +772,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -814,6 +788,32 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1129,15 +1129,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{542763A0-908A-4A86-B48C-F22A6103A71B}" name="CO2_Agricultura_Chile3" displayName="CO2_Agricultura_Chile3" ref="A2:F299" totalsRowShown="0" headerRowDxfId="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{542763A0-908A-4A86-B48C-F22A6103A71B}" name="CO2_Agricultura_Chile3" displayName="CO2_Agricultura_Chile3" ref="A2:F299" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A2:F299" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{EDFE7A38-641B-494A-8910-C33A357024C3}" name="Año" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{EDFE7A38-641B-494A-8910-C33A357024C3}" name="Año" dataDxfId="5"/>
     <tableColumn id="14" xr3:uid="{02F8B638-4A46-4983-93C7-E44ECACBB250}" name="Sector" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{06A1A192-2A07-4AD1-83F1-4056BE6BB6C4}" name="Proceso" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{9C5D1406-D0EB-4EEA-AB79-84EEAE7339B4}" name="Gas" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{06A1A192-2A07-4AD1-83F1-4056BE6BB6C4}" name="Proceso" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{9C5D1406-D0EB-4EEA-AB79-84EEAE7339B4}" name="Gas" dataDxfId="2"/>
     <tableColumn id="16" xr3:uid="{F445F3F8-4CF9-4B56-9A61-943541AA31F3}" name="Emisiones (kton CO2)" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{FD7EDAA8-04D6-4326-8AA5-B09E3FBF4DE1}" name="Emisiones (kton CO2eq)" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{FD7EDAA8-04D6-4326-8AA5-B09E3FBF4DE1}" name="Emisiones (kton CO2eq)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1463,20 +1463,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2571,38 +2571,38 @@
     <col min="2" max="2" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>